<commit_message>
Linear Vertical and updated (Z) added
Programs for plot comparison and std deviation for linear Vertical and Linear updated added.
</commit_message>
<xml_diff>
--- a/Linear/Standard_Deviation Lin.xlsx
+++ b/Linear/Standard_Deviation Lin.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,22 +460,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1034469953152863</v>
+        <v>0.1182059035512639</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1711228794993377</v>
+        <v>0.1376223264721769</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1051269784595163</v>
+        <v>0.05956167798364864</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08616919502045743</v>
+        <v>0.09371153272630643</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1598638593149164</v>
+        <v>0.08474262395795443</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0645806176381592</v>
+        <v>0.06945385870491867</v>
       </c>
     </row>
     <row r="4">
@@ -485,22 +485,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1002663528393916</v>
+        <v>0.03136035073482118</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1356507392760177</v>
+        <v>0.03429929960042005</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1271339080510651</v>
+        <v>0.03346630074544385</v>
       </c>
       <c r="E4" t="n">
-        <v>0.07369798198355301</v>
+        <v>0.02629950238907533</v>
       </c>
       <c r="F4" t="n">
-        <v>0.185042684636576</v>
+        <v>0.02820561540189194</v>
       </c>
       <c r="G4" t="n">
-        <v>0.08335949877338682</v>
+        <v>0.0250851446287112</v>
       </c>
     </row>
     <row r="5">
@@ -510,22 +510,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1008264734410491</v>
+        <v>0.1034469953152863</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1231727714504943</v>
+        <v>0.1711228794993377</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1183008443928716</v>
+        <v>0.1051269784595163</v>
       </c>
       <c r="E5" t="n">
-        <v>0.07530479261559697</v>
+        <v>0.08616919502045743</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1853685584745446</v>
+        <v>0.1598638593149164</v>
       </c>
       <c r="G5" t="n">
-        <v>0.08176751009661042</v>
+        <v>0.0645806176381592</v>
       </c>
     </row>
     <row r="6">
@@ -535,21 +535,71 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>0.1002663528393916</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1356507392760177</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1271339080510651</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.07369798198355301</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.185042684636576</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.08335949877338682</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Std_dev Rect5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1008264734410491</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1231727714504943</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1183008443928716</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.07530479261559697</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.1853685584745446</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.08176751009661042</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Std_dev Rect6</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>0.07919348390661737</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C8" t="n">
         <v>0.1380466719077388</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D8" t="n">
         <v>0.1073543596419539</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E8" t="n">
         <v>0.0817545268920974</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F8" t="n">
         <v>0.1438396245088136</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G8" t="n">
         <v>0.08355746418490252</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Linear experiment updated for new traces
</commit_message>
<xml_diff>
--- a/Linear/Standard_Deviation Lin.xlsx
+++ b/Linear/Standard_Deviation Lin.xlsx
@@ -510,22 +510,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1034469953152863</v>
+        <v>0.2560897945784967</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1711228794993377</v>
+        <v>0.1922302243704833</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1051269784595163</v>
+        <v>0.1453653151772641</v>
       </c>
       <c r="E5" t="n">
-        <v>0.08616919502045739</v>
+        <v>0.1929223575287684</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1598638593149165</v>
+        <v>0.2240464861714938</v>
       </c>
       <c r="G5" t="n">
-        <v>0.06458061763815925</v>
+        <v>0.2544840169573067</v>
       </c>
     </row>
     <row r="6">
@@ -535,22 +535,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1002663528393917</v>
+        <v>0.2770267008588849</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1356507392760177</v>
+        <v>0.1605440980871795</v>
       </c>
       <c r="D6" t="n">
-        <v>0.127133908051065</v>
+        <v>0.1369792959557058</v>
       </c>
       <c r="E6" t="n">
-        <v>0.07369798198355301</v>
+        <v>0.208388836430242</v>
       </c>
       <c r="F6" t="n">
-        <v>0.185042684636576</v>
+        <v>0.2068473773143613</v>
       </c>
       <c r="G6" t="n">
-        <v>0.08335949877338682</v>
+        <v>0.2132499575263846</v>
       </c>
     </row>
     <row r="7">
@@ -560,22 +560,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1008264734410491</v>
+        <v>0.1748995270691545</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1231727714504943</v>
+        <v>0.08298676030387352</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1183008443928715</v>
+        <v>0.09247763512786311</v>
       </c>
       <c r="E7" t="n">
-        <v>0.07530479261559696</v>
+        <v>0.1442451350674593</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1853685584745448</v>
+        <v>0.1477468036115866</v>
       </c>
       <c r="G7" t="n">
-        <v>0.08176751009661043</v>
+        <v>0.1175250756782335</v>
       </c>
     </row>
     <row r="8">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.07919348390661732</v>
+        <v>0.1396381204092653</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1380466719077388</v>
+        <v>0.03970428935642073</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1073543596419539</v>
+        <v>0.05091816180503488</v>
       </c>
       <c r="E8" t="n">
-        <v>0.08175452689209742</v>
+        <v>0.1933786134269216</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1438396245088137</v>
+        <v>0.1249432911345317</v>
       </c>
       <c r="G8" t="n">
-        <v>0.08355746418490248</v>
+        <v>0.1813139052758002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Linear experiment updated for sim and real traces
</commit_message>
<xml_diff>
--- a/Linear/Standard_Deviation Lin.xlsx
+++ b/Linear/Standard_Deviation Lin.xlsx
@@ -510,22 +510,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2560897945784967</v>
+        <v>0.00222625182058704</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1922302243704833</v>
+        <v>0.001569787117169649</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1453653151772641</v>
+        <v>0.001325577226074754</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1929223575287684</v>
+        <v>0.0018572632978132</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2240464861714938</v>
+        <v>0.001738689689759812</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2544840169573067</v>
+        <v>0.00157962338536876</v>
       </c>
     </row>
     <row r="6">
@@ -535,22 +535,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2770267008588849</v>
+        <v>0.001991614944459785</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1605440980871795</v>
+        <v>0.001291350478748593</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1369792959557058</v>
+        <v>0.001244958982792127</v>
       </c>
       <c r="E6" t="n">
-        <v>0.208388836430242</v>
+        <v>0.001218624070470127</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2068473773143613</v>
+        <v>0.001429028797842887</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2132499575263846</v>
+        <v>0.001122456285256862</v>
       </c>
     </row>
     <row r="7">
@@ -560,22 +560,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1748995270691545</v>
+        <v>0.004350634231105001</v>
       </c>
       <c r="C7" t="n">
-        <v>0.08298676030387352</v>
+        <v>0.004538637975386308</v>
       </c>
       <c r="D7" t="n">
-        <v>0.09247763512786311</v>
+        <v>0.003314520384202478</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1442451350674593</v>
+        <v>0.004140273757784414</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1477468036115866</v>
+        <v>0.00426150058787862</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1175250756782335</v>
+        <v>0.003246756277608157</v>
       </c>
     </row>
     <row r="8">
@@ -585,22 +585,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1396381204092653</v>
+        <v>0.0005953469904289718</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03970428935642073</v>
+        <v>0.0004268645716496332</v>
       </c>
       <c r="D8" t="n">
-        <v>0.05091816180503488</v>
+        <v>0.0005533050419349652</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1933786134269216</v>
+        <v>0.0007503747311340246</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1249432911345317</v>
+        <v>0.0007675501956847752</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1813139052758002</v>
+        <v>0.0006647402874995507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>